<commit_message>
se realiza ajuste del DataExcelModels y se quitan los datos quemados del portinPrepago
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla3\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3021AC89-A855-4E15-8047-163F8C3D61E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37883F6F-3884-4F86-9F6A-1A7746BE8757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="75">
   <si>
     <t>MSIDN</t>
   </si>
@@ -151,9 +151,6 @@
     <t>3043209819</t>
   </si>
   <si>
-    <t>732111324707277</t>
-  </si>
-  <si>
     <t>3043209868</t>
   </si>
   <si>
@@ -248,6 +245,12 @@
   </si>
   <si>
     <t>621218573</t>
+  </si>
+  <si>
+    <t>732111324707278</t>
+  </si>
+  <si>
+    <t xml:space="preserve">732111324707277 </t>
   </si>
 </sst>
 </file>
@@ -666,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B13"/>
+      <selection activeCell="A13" sqref="A13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -707,7 +710,7 @@
         <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1">
@@ -715,7 +718,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>28</v>
@@ -736,7 +739,7 @@
         <v>27</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1">
@@ -767,13 +770,13 @@
         <v>11</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1">
@@ -790,13 +793,13 @@
         <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1">
@@ -841,19 +844,19 @@
         <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1">
@@ -861,7 +864,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>36</v>
@@ -870,19 +873,19 @@
         <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1">
@@ -890,7 +893,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>37</v>
@@ -899,19 +902,19 @@
         <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1">
@@ -919,7 +922,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
@@ -933,7 +936,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>40</v>
@@ -947,13 +950,27 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3043209863</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -972,10 +989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D188C588-523E-4AEF-A066-FA5DCECDB773}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C14" sqref="C14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1013,7 +1030,7 @@
         <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1">
@@ -1042,7 +1059,7 @@
         <v>27</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1">
@@ -1061,10 +1078,10 @@
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
@@ -1073,18 +1090,18 @@
         <v>11</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
@@ -1096,18 +1113,18 @@
         <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>14</v>
@@ -1124,7 +1141,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>17</v>
@@ -1147,19 +1164,19 @@
         <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1">
@@ -1167,7 +1184,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>36</v>
@@ -1176,19 +1193,19 @@
         <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1">
@@ -1196,7 +1213,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>37</v>
@@ -1205,19 +1222,19 @@
         <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1">
@@ -1225,7 +1242,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
@@ -1239,7 +1256,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>40</v>
@@ -1253,13 +1270,27 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>41</v>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3043209863</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>